<commit_message>
Refactoring to comply with PageObject approach, added more logs
</commit_message>
<xml_diff>
--- a/qaseChecklist.xlsx
+++ b/qaseChecklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw5_QaseAutomation\hw5_qaseAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1C6BBE-240D-4E2B-938C-FE6B60EF71B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50F7282-C542-442E-AF85-BAC876CE785F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Статус</t>
   </si>
@@ -108,10 +108,13 @@
     <t>E2E</t>
   </si>
   <si>
-    <t>Create 3 Test Cases and add to Test Plan</t>
-  </si>
-  <si>
     <t>In Qase</t>
+  </si>
+  <si>
+    <t>Automated</t>
+  </si>
+  <si>
+    <t>Create 2 Test Cases and add to Test Plan</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,7 +560,7 @@
     <col min="1" max="1" width="15.81640625" customWidth="1"/>
     <col min="2" max="2" width="46.36328125" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
     <col min="5" max="5" width="35.08984375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -588,7 +591,9 @@
       <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -599,7 +604,9 @@
       <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -610,7 +617,9 @@
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -621,7 +630,9 @@
       <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -654,7 +665,9 @@
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -678,7 +691,9 @@
       <c r="C10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -698,7 +713,9 @@
       <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -709,7 +726,9 @@
       <c r="C13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -717,7 +736,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Creating Test Plan model and base Test Plan tests
</commit_message>
<xml_diff>
--- a/qaseChecklist.xlsx
+++ b/qaseChecklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw5_QaseAutomation\hw5_qaseAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50F7282-C542-442E-AF85-BAC876CE785F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796D968F-1DCA-423E-9182-F85A58484811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Статус</t>
   </si>
@@ -114,7 +114,13 @@
     <t>Automated</t>
   </si>
   <si>
-    <t>Create 2 Test Cases and add to Test Plan</t>
+    <t>Create 2 Test Cases and add to Test Plan as Suite</t>
+  </si>
+  <si>
+    <t>Create 3 Test Cases in 1 Suite and add 2 to Test Plan</t>
+  </si>
+  <si>
+    <t>To do</t>
   </si>
 </sst>
 </file>
@@ -200,21 +206,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,7 +560,7 @@
   <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -585,7 +593,7 @@
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -598,7 +606,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -611,7 +619,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -624,7 +632,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -643,10 +651,10 @@
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -658,8 +666,8 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -671,8 +679,8 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -684,8 +692,8 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -697,14 +705,14 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -719,8 +727,8 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -732,34 +740,41 @@
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D17" s="9"/>
       <c r="E17"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Created Test Cases for Test Plans CRUD
</commit_message>
<xml_diff>
--- a/qaseChecklist.xlsx
+++ b/qaseChecklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw5_QaseAutomation\hw5_qaseAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796D968F-1DCA-423E-9182-F85A58484811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7CC681-D545-43CA-A424-C75BB8C55716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>Статус</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>E2E</t>
-  </si>
-  <si>
-    <t>In Qase</t>
   </si>
   <si>
     <t>Automated</t>
@@ -188,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -220,9 +217,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +554,7 @@
   <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -661,7 +655,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="8"/>
     </row>
@@ -674,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -687,7 +681,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="8"/>
     </row>
@@ -700,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="8"/>
     </row>
@@ -722,7 +716,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="8"/>
     </row>
@@ -735,7 +729,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="8"/>
     </row>
@@ -744,26 +738,26 @@
         <v>22</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="12" t="s">
-        <v>26</v>
+      <c r="B15" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="8"/>
     </row>

</xml_diff>

<commit_message>
Update checklist and Logging configuration
</commit_message>
<xml_diff>
--- a/qaseChecklist.xlsx
+++ b/qaseChecklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw5_QaseAutomation\hw5_qaseAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7CC681-D545-43CA-A424-C75BB8C55716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAF6A66-3BBC-4DD7-9005-034466BD7EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>Статус</t>
   </si>
@@ -112,12 +112,6 @@
   </si>
   <si>
     <t>Create 2 Test Cases and add to Test Plan as Suite</t>
-  </si>
-  <si>
-    <t>Create 3 Test Cases in 1 Suite and add 2 to Test Plan</t>
-  </si>
-  <si>
-    <t>To do</t>
   </si>
 </sst>
 </file>
@@ -554,7 +548,7 @@
   <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,21 +738,15 @@
         <v>22</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Create WebAPI Tests: CRUD Test Cases, CRUD Test Plans
</commit_message>
<xml_diff>
--- a/qaseChecklist.xlsx
+++ b/qaseChecklist.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw5_QaseAutomation\hw5_qaseAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAF6A66-3BBC-4DD7-9005-034466BD7EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C65A40B-F543-40BC-9AD5-9BBDBE05FFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Тест-кейсы на автоматизацию" sheetId="5" r:id="rId1"/>
-    <sheet name="Фиксы" sheetId="2" r:id="rId2"/>
+    <sheet name="WebAPI Automation" sheetId="6" r:id="rId2"/>
+    <sheet name="Фиксы" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="34">
   <si>
     <t>Статус</t>
   </si>
@@ -112,6 +113,33 @@
   </si>
   <si>
     <t>Create 2 Test Cases and add to Test Plan as Suite</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>Before-After</t>
+  </si>
+  <si>
+    <t>Create Mock Cases before test</t>
+  </si>
+  <si>
+    <t>Delete Mock cases after test</t>
+  </si>
+  <si>
+    <t>Проверки</t>
+  </si>
+  <si>
+    <t>Code, Body</t>
+  </si>
+  <si>
+    <t>Code 200</t>
+  </si>
+  <si>
+    <t>Code 204</t>
+  </si>
+  <si>
+    <t>Пока костыльно</t>
   </si>
 </sst>
 </file>
@@ -135,12 +163,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -179,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -212,11 +252,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -269,14 +384,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6998AABF-FC77-48A5-8AA0-30BE1579D29E}" name="Table13" displayName="Table13" ref="A1:E17" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6998AABF-FC77-48A5-8AA0-30BE1579D29E}" name="Table13" displayName="Table13" ref="A1:E17" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7">
   <autoFilter ref="A1:E17" xr:uid="{FE89EFD3-F5E6-427A-A4AE-782233C9841D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D5D7C9F8-4B1F-412C-8FF2-6F8DC0F54C75}" name="Модуль"/>
-    <tableColumn id="3" xr3:uid="{F9A68072-5A64-4BB2-9A67-2824EE1D1EDF}" name="Тест-кейс" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{7081D3CF-0355-45A9-BF8E-AAF1ACAAF437}" name="Тип теста" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{F9A68072-5A64-4BB2-9A67-2824EE1D1EDF}" name="Тест-кейс" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{7081D3CF-0355-45A9-BF8E-AAF1ACAAF437}" name="Тип теста" dataDxfId="5"/>
     <tableColumn id="9" xr3:uid="{0E2992C3-5DDE-4610-88AA-E9D665C806EF}" name="Статус"/>
     <tableColumn id="10" xr3:uid="{52A2EBC7-61BB-4F6A-9629-91DC3BB12D6C}" name="Комментарии"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57DA372B-DEC7-4741-A426-1FAD90011043}" name="Table132" displayName="Table132" ref="A1:F13" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3">
+  <autoFilter ref="A1:F13" xr:uid="{FE89EFD3-F5E6-427A-A4AE-782233C9841D}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E0720D68-9FE0-49AD-9176-53A57CACE71F}" name="Модуль"/>
+    <tableColumn id="3" xr3:uid="{493935B4-1EC4-47B6-BC50-4821428D3E5A}" name="Тест-кейс" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{73A43B7E-E8E0-4321-9B05-6F55525415FB}" name="Тип теста" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{11700686-ED52-47DD-811B-6F3971EEA48A}" name="Проверки" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{6026B490-FBB2-44B9-A271-91E0121AA38F}" name="Статус"/>
+    <tableColumn id="10" xr3:uid="{E51CAA94-3C43-420D-B395-BE85FD4CE250}" name="Комментарии"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -547,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B755BA-AB1D-4BD0-B742-796615240701}">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1105,6 +1235,652 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25109945-646A-47AE-9D8B-072C88249BD3}">
+  <dimension ref="A1:F95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="46.36328125" style="3" customWidth="1"/>
+    <col min="3" max="4" width="15.36328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="35.08984375" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
+      <c r="B8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="9"/>
+      <c r="B9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+      <c r="B10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C68"/>
+      <c r="D68"/>
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C69"/>
+      <c r="D69"/>
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C70"/>
+      <c r="D70"/>
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C72"/>
+      <c r="D72"/>
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C73"/>
+      <c r="D73"/>
+      <c r="F73"/>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C74"/>
+      <c r="D74"/>
+      <c r="F74"/>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C75"/>
+      <c r="D75"/>
+      <c r="F75"/>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="F76"/>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="F78"/>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="F79"/>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="F80"/>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="F81"/>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="F82"/>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="F92"/>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="F93"/>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="F95"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D8DF8D-3BDE-4455-81F1-A528355B1E3F}">
   <dimension ref="A1:D8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added reading test case via API
</commit_message>
<xml_diff>
--- a/qaseChecklist.xlsx
+++ b/qaseChecklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw5_QaseAutomation\hw5_qaseAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C65A40B-F543-40BC-9AD5-9BBDBE05FFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECD6813-D4C2-43F4-8296-6EBEA25CB06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
   <si>
     <t>Статус</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>Code 200</t>
-  </si>
-  <si>
-    <t>Code 204</t>
   </si>
   <si>
     <t>Пока костыльно</t>
@@ -178,7 +175,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -269,6 +266,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1239,7 +1239,7 @@
   <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1304,7 +1304,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1331,8 +1331,8 @@
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>32</v>
+      <c r="D5" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>25</v>
@@ -1357,7 +1357,7 @@
       <c r="C7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -1373,13 +1373,15 @@
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="17" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
@@ -1389,7 +1391,7 @@
       <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="16" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -1405,8 +1407,8 @@
       <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>32</v>
+      <c r="D10" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>25</v>
@@ -1431,7 +1433,7 @@
       <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="7" t="s">
@@ -1446,7 +1448,7 @@
       <c r="C13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="18" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="14" t="s">

</xml_diff>